<commit_message>
refector:Excel Test get data code optimize
</commit_message>
<xml_diff>
--- a/src/main/java/com/tutorialninja/qa/testdata/tutorialNinjaTestData.xlsx
+++ b/src/main/java/com/tutorialninja/qa/testdata/tutorialNinjaTestData.xlsx
@@ -7,18 +7,47 @@
     <workbookView xWindow="240" yWindow="60" windowWidth="20055" windowHeight="7950"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Login" sheetId="2" r:id="rId1"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="6">
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>testdemo2@gmail.com</t>
+  </si>
+  <si>
+    <t>Admin@123</t>
+  </si>
+  <si>
+    <t>testdemo3@gmail.com</t>
+  </si>
+  <si>
+    <t>testdemo4@gmail.com</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+  <fonts count="2">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -46,8 +75,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -342,38 +372,52 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="38.140625" customWidth="1"/>
+    <col min="2" max="2" width="14.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>